<commit_message>
Steven map hernieuwd (alweer)
</commit_message>
<xml_diff>
--- a/Barroc IT - Documentatie/Steven/Notulen base.xlsx
+++ b/Barroc IT - Documentatie/Steven/Notulen base.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Afwezig:</t>
   </si>
@@ -42,28 +42,16 @@
     <t>2 Mededelingen</t>
   </si>
   <si>
-    <t>9 Rondvraag</t>
-  </si>
-  <si>
-    <t>8 Vastellen volgende vergadering: week 12</t>
-  </si>
-  <si>
-    <t>Verslag overleg op</t>
-  </si>
-  <si>
-    <t>3 Notulen vorige vergadering (d.d. 25-8-2014 tabblad)</t>
-  </si>
-  <si>
     <t>Aanwezig: Tom Smits, Steven Logghe, Santino Bonora</t>
   </si>
   <si>
     <t>Notulen aan: Fer van Krimpen, Twig van Beek</t>
   </si>
   <si>
-    <t>Agenda moet opnieuw worden opgedeelt</t>
-  </si>
-  <si>
-    <t>10 vorige vergadering</t>
+    <t>3 Vaststellen volgende vergaderpunt</t>
+  </si>
+  <si>
+    <t>Verslag overleg op …………..</t>
   </si>
 </sst>
 </file>
@@ -101,6 +89,7 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -206,23 +195,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -579,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +582,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -614,10 +603,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
+        <v>8</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="3"/>
@@ -637,8 +626,8 @@
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="3"/>
@@ -656,10 +645,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
+        <v>9</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="3"/>
@@ -724,12 +713,10 @@
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
@@ -747,7 +734,7 @@
       <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="8"/>
@@ -768,8 +755,8 @@
       <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>11</v>
+      <c r="A9" s="21" t="s">
+        <v>10</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -788,8 +775,8 @@
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
     </row>
-    <row r="10" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -807,103 +794,85 @@
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
     </row>
-    <row r="11" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>9</v>
-      </c>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
       <c r="B14" s="16"/>
       <c r="C14" s="14"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
-        <v>8</v>
-      </c>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>15</v>
-      </c>
+      <c r="A16" s="23"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
-        <v>11</v>
-      </c>
+      <c r="A17" s="23"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
-        <v>12</v>
-      </c>
+      <c r="A18" s="23"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
-        <v>13</v>
-      </c>
+      <c r="A19" s="23"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
-        <v>14</v>
-      </c>
+      <c r="A20" s="23"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="19">
-        <v>15</v>
-      </c>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A22" s="19">
-        <v>16</v>
-      </c>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="15"/>
@@ -986,18 +955,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1050,14 +1019,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79336D9A-F347-4BF9-A03C-2F519BF74106}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F91946DA-1D0C-4852-AC5F-029A4620CB68}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1067,6 +1028,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79336D9A-F347-4BF9-A03C-2F519BF74106}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>